<commit_message>
porty1: Scrum Backlog and Planing Sprint 1
</commit_message>
<xml_diff>
--- a/doc/task10/scrum_teamgreen.xlsx
+++ b/doc/task10/scrum_teamgreen.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yannis\workspace\ch.bfh.btx8081.w2015.green\doc\task10\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2436" windowWidth="16404" windowHeight="5316" activeTab="2"/>
   </bookViews>
@@ -12,13 +17,12 @@
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
-  <oleSize ref="A1:N9"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -38,24 +42,12 @@
     <t>high</t>
   </si>
   <si>
-    <t>medium</t>
-  </si>
-  <si>
     <t>low</t>
   </si>
   <si>
     <t>waiting</t>
   </si>
   <si>
-    <t>work in progress</t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>cancelled</t>
-  </si>
-  <si>
     <t>Owner</t>
   </si>
   <si>
@@ -71,30 +63,9 @@
     <t>Effort Actual</t>
   </si>
   <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t>Hans</t>
-  </si>
-  <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Jennifer</t>
-  </si>
-  <si>
     <t>Database</t>
   </si>
   <si>
-    <t>UI, Controller</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Main Window</t>
-  </si>
-  <si>
     <t>Effort Plan Original</t>
   </si>
   <si>
@@ -164,25 +135,99 @@
     <t>Record a new case. Add diagnosis. Add Treatment. Edit Case.</t>
   </si>
   <si>
-    <t>Data model for patient record needs to be created based on standard sql.</t>
-  </si>
-  <si>
     <t>Patient</t>
   </si>
   <si>
-    <t>Data model for doctor login record needs to be created based on standard sql.</t>
-  </si>
-  <si>
     <t>20h</t>
   </si>
   <si>
-    <t>65h</t>
-  </si>
-  <si>
-    <t>35h</t>
-  </si>
-  <si>
-    <t>Create class Patient</t>
+    <t>Manuel Pfister</t>
+  </si>
+  <si>
+    <t>55h</t>
+  </si>
+  <si>
+    <t>75h</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Pfister</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>User Interface for Login</t>
+  </si>
+  <si>
+    <t>Login functionality</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>Data model for patient record</t>
+  </si>
+  <si>
+    <t>Data model for doctor login</t>
+  </si>
+  <si>
+    <t>User Interface</t>
+  </si>
+  <si>
+    <t>User Interface needs 
+to be designed</t>
+  </si>
+  <si>
+    <t>create new Patient,
+ edit Data, save Data</t>
+  </si>
+  <si>
+    <t>Data model for 
+Message</t>
+  </si>
+  <si>
+    <t>create/send/receive 
+Message, delete Message</t>
+  </si>
+  <si>
+    <t>Data model for Case, 
+Diagnosis, Treatment and Medication</t>
+  </si>
+  <si>
+    <t>Functionality for 
+new Case, new Diagnosis, new Treatment, edit Treatment, delete Treatment, edit Diagnosis, new Medication, edit Medication and Delete Medication</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Application GUI needs 
+to be designed and prepared for further steps</t>
+  </si>
+  <si>
+    <t>Effort (h) Plan Original</t>
+  </si>
+  <si>
+    <t>Effort (h) Plan Updated</t>
+  </si>
+  <si>
+    <t>Mele</t>
+  </si>
+  <si>
+    <t>Vladi</t>
+  </si>
+  <si>
+    <t>Ramos</t>
+  </si>
+  <si>
+    <t>Portmann</t>
+  </si>
+  <si>
+    <t>Mele
+Portmann</t>
   </si>
 </sst>
 </file>
@@ -269,14 +314,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -314,9 +362,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -351,7 +399,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -386,7 +434,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -563,7 +611,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,42 +625,46 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -620,10 +672,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -643,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -652,13 +704,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
@@ -669,25 +721,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -695,25 +744,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -721,42 +767,26 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3"/>
+        <v>7</v>
+      </c>
+    </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H9" t="s">
-        <v>10</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -766,10 +796,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -777,7 +807,7 @@
     <col min="1" max="1" width="4.77734375" customWidth="1"/>
     <col min="2" max="2" width="6.21875" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" customWidth="1"/>
     <col min="7" max="7" width="9.77734375" customWidth="1"/>
@@ -793,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -802,25 +832,25 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>4</v>
@@ -828,217 +858,382 @@
     </row>
     <row r="2" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
       </c>
       <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
       </c>
       <c r="I3">
-        <v>8</v>
-      </c>
-      <c r="J3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s">
         <v>5</v>
       </c>
       <c r="I4">
-        <v>16</v>
-      </c>
-      <c r="J4">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
+        <v>1.3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>2.1</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5">
-        <v>4</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="H6" t="s">
         <v>5</v>
       </c>
       <c r="I6">
-        <v>8</v>
-      </c>
-      <c r="J6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8">
+        <v>15</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3.1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3.2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
       <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" t="s">
-        <v>7</v>
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3.3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="E11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11">
+        <v>7</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" t="s">
         <v>5</v>
       </c>
-      <c r="L11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" t="s">
-        <v>6</v>
+      <c r="I12">
+        <v>20</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>4.2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13">
+        <v>30</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
       <c r="L13" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>4.3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14">
+        <v>44</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1051,7 +1246,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1063,16 +1258,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1083,10 +1278,10 @@
         <v>42327</v>
       </c>
       <c r="C2">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D2">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1097,10 +1292,10 @@
         <v>42327</v>
       </c>
       <c r="C3">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="D3">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1111,10 +1306,10 @@
         <v>42327</v>
       </c>
       <c r="C4">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D4">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>